<commit_message>
update parts order name
</commit_message>
<xml_diff>
--- a/Projects/Cupboard Parts/output.xlsx
+++ b/Projects/Cupboard Parts/output.xlsx
@@ -499,23 +499,26 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CLASSIC KICK</t>
+          <t>DOOR</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>41 7/8 X 4</t>
+          <t>8 7/8 X 26 1/2</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>47 7/8 X 4</t>
-        </is>
+          <t>11 7/8 X 31 7/8</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
       </c>
       <c r="D4" t="n">
         <v>2</v>
@@ -524,19 +527,19 @@
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>59 7/8 X 4</t>
+          <t>11 7/8 X 26 1/2</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="C6" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7"/>
@@ -544,75 +547,72 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DOOR</t>
+          <t>DRAWER</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>8 7/8 X 26 1/2</t>
+          <t>11 7/8 X 8 3/4</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="D9" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>11 7/8 X 31 7/8</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>2</v>
-      </c>
-      <c r="D10" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>11 7/8 X 26 1/2</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="C12" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13"/>
-    <row r="14"/>
+      <c r="C10" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>CLASSIC KICK</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>41 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>47 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>2</v>
+      </c>
+    </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>DRAWER</t>
-        </is>
-      </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>11 7/8 X 8 3/4</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>6</v>
+          <t>59 7/8 X 4</t>
+        </is>
       </c>
       <c r="D15" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="C16" s="2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17"/>
@@ -710,90 +710,93 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CLASSIC KICK</t>
+          <t>DOOR</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>14 7/8 X 4</t>
+          <t>8 7/8 X 26 1/2</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="inlineStr">
         <is>
-          <t>23 7/8 X 4</t>
-        </is>
+          <t>11 7/8 X 26 1/2</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>2</v>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="inlineStr">
         <is>
-          <t>29 7/8 X 4</t>
-        </is>
-      </c>
-      <c r="F30" t="n">
-        <v>1</v>
+          <t>11 7/8 X 19 1/2</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="inlineStr">
         <is>
-          <t>35 7/8 X 4</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>1</v>
+          <t>11 7/8 X 17 9/16</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="inlineStr">
         <is>
-          <t>41 7/8 X 4</t>
+          <t>14 7/8 X 17 9/16</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="inlineStr">
         <is>
-          <t>59 7/8 X 4</t>
+          <t>14 7/8 X 26 1/2</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="inlineStr">
         <is>
-          <t>71 7/8 X 4</t>
+          <t>14 7/8 X 44 1/8</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="C35" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36"/>
@@ -801,167 +804,164 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>DOOR</t>
+          <t>DRAWER</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>8 7/8 X 26 1/2</t>
-        </is>
+          <t>11 7/8 X 8 3/4</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>3</v>
       </c>
       <c r="F38" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="inlineStr">
         <is>
-          <t>11 7/8 X 17 9/16</t>
-        </is>
-      </c>
-      <c r="F39" t="n">
-        <v>4</v>
+          <t>11 7/8 X 9 11/16</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="inlineStr">
         <is>
-          <t>11 7/8 X 26 1/2</t>
-        </is>
-      </c>
-      <c r="C40" t="n">
-        <v>2</v>
-      </c>
-      <c r="D40" t="n">
+          <t>23 7/8 X 8 3/4</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="inlineStr">
         <is>
-          <t>11 7/8 X 19 1/2</t>
-        </is>
-      </c>
-      <c r="E41" t="n">
-        <v>2</v>
+          <t>29 7/8 X 8 3/4</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="inlineStr">
         <is>
-          <t>14 7/8 X 17 9/16</t>
-        </is>
-      </c>
-      <c r="F42" t="n">
-        <v>8</v>
+          <t>35 7/8 X 6 15/16</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="43">
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>14 7/8 X 44 1/8</t>
-        </is>
-      </c>
-      <c r="F43" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>14 7/8 X 26 1/2</t>
-        </is>
-      </c>
-      <c r="F44" t="n">
+      <c r="C43" s="2" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="45">
-      <c r="C45" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D45" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E45" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F45" s="2" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46"/>
-    <row r="47"/>
+      <c r="D43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F43" s="2" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>CLASSIC KICK</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>14 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>23 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>1</v>
+      </c>
+    </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>DRAWER</t>
-        </is>
-      </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>11 7/8 X 9 11/16</t>
-        </is>
-      </c>
-      <c r="E48" t="n">
-        <v>2</v>
+          <t>29 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="inlineStr">
         <is>
-          <t>11 7/8 X 8 3/4</t>
+          <t>35 7/8 X 4</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>3</v>
-      </c>
-      <c r="F49" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="inlineStr">
         <is>
-          <t>23 7/8 X 8 3/4</t>
+          <t>41 7/8 X 4</t>
         </is>
       </c>
       <c r="F50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="inlineStr">
         <is>
-          <t>29 7/8 X 8 3/4</t>
+          <t>59 7/8 X 4</t>
         </is>
       </c>
       <c r="F51" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="inlineStr">
         <is>
-          <t>35 7/8 X 6 15/16</t>
-        </is>
-      </c>
-      <c r="E52" t="n">
-        <v>1</v>
+          <t>71 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="53">
       <c r="C53" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D53" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E53" s="2" t="n">
-        <v>3</v>
-      </c>
       <c r="F53" s="2" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54"/>
@@ -1140,17 +1140,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CLASSIC KICK</t>
+          <t>DOOR</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>41 7/8 X 4</t>
+          <t>8 7/8 X 26 1/2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">NATURAL - 1
+          <t xml:space="preserve">NATURAL - 2
 </t>
         </is>
       </c>
@@ -1158,7 +1158,13 @@
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>47 7/8 X 4</t>
+          <t>11 7/8 X 31 7/8</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NATURAL - 2
+</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1171,22 +1177,22 @@
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>59 7/8 X 4</t>
+          <t>11 7/8 X 26 1/2</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">AHM 3700 - 1
+          <t xml:space="preserve">AHM 3700 - 8
 </t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="C6" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7"/>
@@ -1194,93 +1200,87 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DOOR</t>
+          <t>DRAWER</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>8 7/8 X 26 1/2</t>
+          <t>11 7/8 X 8 3/4</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">NATURAL - 2
+          <t xml:space="preserve">NATURAL - 6
+</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHM 3700 - 15
 </t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>11 7/8 X 31 7/8</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NATURAL - 2
-</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
+      <c r="C10" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>CLASSIC KICK</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>41 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NATURAL - 1
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>47 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t xml:space="preserve">AHM 3700 - 2
 </t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>11 7/8 X 26 1/2</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AHM 3700 - 8
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="C12" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13"/>
-    <row r="14"/>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>DRAWER</t>
-        </is>
-      </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>11 7/8 X 8 3/4</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NATURAL - 6
-</t>
+          <t>59 7/8 X 4</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve">AHM 3700 - 15
+          <t xml:space="preserve">AHM 3700 - 1
 </t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="C16" s="2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17"/>
@@ -1387,17 +1387,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CLASSIC KICK</t>
+          <t>DOOR</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>14 7/8 X 4</t>
+          <t>8 7/8 X 26 1/2</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t xml:space="preserve">AHM 10 MATTE - 1
+          <t xml:space="preserve">AHM 80 - 2
 </t>
         </is>
       </c>
@@ -1405,12 +1405,18 @@
     <row r="29">
       <c r="B29" t="inlineStr">
         <is>
-          <t>23 7/8 X 4</t>
+          <t>11 7/8 X 26 1/2</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHM 50 - 2
+</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t xml:space="preserve">AHM 20 MATTE - 1
+          <t xml:space="preserve">AHM 20 MATTE - 2
 </t>
         </is>
       </c>
@@ -1418,12 +1424,12 @@
     <row r="30">
       <c r="B30" t="inlineStr">
         <is>
-          <t>29 7/8 X 4</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AHM 25 - 1
+          <t>11 7/8 X 19 1/2</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHM 10 MATTE - 2
 </t>
         </is>
       </c>
@@ -1431,12 +1437,12 @@
     <row r="31">
       <c r="B31" t="inlineStr">
         <is>
-          <t>35 7/8 X 4</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AHM 50 - 1
+          <t>11 7/8 X 17 9/16</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHM 10 MATTE - 4
 </t>
         </is>
       </c>
@@ -1444,12 +1450,13 @@
     <row r="32">
       <c r="B32" t="inlineStr">
         <is>
-          <t>41 7/8 X 4</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AHM 80 - 1
+          <t>14 7/8 X 17 9/16</t>
+        </is>
+      </c>
+      <c r="F32" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHM 10 MATTE - 4
+AHM 40 - 4
 </t>
         </is>
       </c>
@@ -1457,12 +1464,13 @@
     <row r="33">
       <c r="B33" t="inlineStr">
         <is>
-          <t>59 7/8 X 4</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
+          <t>14 7/8 X 26 1/2</t>
+        </is>
+      </c>
+      <c r="F33" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">AHM 10 MATTE - 1
+AHM 25 - 2
 </t>
         </is>
       </c>
@@ -1470,29 +1478,28 @@
     <row r="34">
       <c r="B34" t="inlineStr">
         <is>
-          <t>71 7/8 X 4</t>
-        </is>
-      </c>
-      <c r="F34" s="3" t="inlineStr">
+          <t>14 7/8 X 44 1/8</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
         <is>
           <t xml:space="preserve">AHM 10 MATTE - 1
-AHM 40 - 1
 </t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="C35" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36"/>
@@ -1500,154 +1507,21 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>DOOR</t>
+          <t>DRAWER</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>8 7/8 X 26 1/2</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AHM 80 - 2
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>11 7/8 X 17 9/16</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AHM 10 MATTE - 4
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>11 7/8 X 26 1/2</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AHM 50 - 2
-</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AHM 20 MATTE - 2
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>11 7/8 X 19 1/2</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AHM 10 MATTE - 2
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>14 7/8 X 17 9/16</t>
-        </is>
-      </c>
-      <c r="F42" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AHM 10 MATTE - 4
-AHM 40 - 4
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>14 7/8 X 44 1/8</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AHM 10 MATTE - 1
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>14 7/8 X 26 1/2</t>
-        </is>
-      </c>
-      <c r="F44" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AHM 10 MATTE - 1
-AHM 25 - 2
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="C45" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D45" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E45" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F45" s="2" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>DRAWER</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>11 7/8 X 9 11/16</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AHM 10 MATTE - 2
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="B49" t="inlineStr">
-        <is>
           <t>11 7/8 X 8 3/4</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t xml:space="preserve">AHM 50 - 3
 </t>
         </is>
       </c>
-      <c r="F49" s="3" t="inlineStr">
+      <c r="F38" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">AHM 10 MATTE - 6
 AHM 40 - 3
@@ -1656,15 +1530,141 @@
         </is>
       </c>
     </row>
+    <row r="39">
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>11 7/8 X 9 11/16</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHM 10 MATTE - 2
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>23 7/8 X 8 3/4</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHM 10 MATTE - 2
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>29 7/8 X 8 3/4</t>
+        </is>
+      </c>
+      <c r="F41" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHM 10 MATTE - 2
+AHM 40 - 2
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>35 7/8 X 6 15/16</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHM 10 MATTE - 1
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="C43" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F43" s="2" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>CLASSIC KICK</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>14 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHM 10 MATTE - 1
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>23 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHM 20 MATTE - 1
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>29 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHM 25 - 1
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>35 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHM 50 - 1
+</t>
+        </is>
+      </c>
+    </row>
     <row r="50">
       <c r="B50" t="inlineStr">
         <is>
-          <t>23 7/8 X 8 3/4</t>
+          <t>41 7/8 X 4</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t xml:space="preserve">AHM 10 MATTE - 2
+          <t xml:space="preserve">AHM 80 - 1
 </t>
         </is>
       </c>
@@ -1672,13 +1672,12 @@
     <row r="51">
       <c r="B51" t="inlineStr">
         <is>
-          <t>29 7/8 X 8 3/4</t>
-        </is>
-      </c>
-      <c r="F51" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AHM 10 MATTE - 2
-AHM 40 - 2
+          <t>59 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHM 10 MATTE - 1
 </t>
         </is>
       </c>
@@ -1686,28 +1685,29 @@
     <row r="52">
       <c r="B52" t="inlineStr">
         <is>
-          <t>35 7/8 X 6 15/16</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
+          <t>71 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="F52" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">AHM 10 MATTE - 1
+AHM 40 - 1
 </t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="C53" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D53" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E53" s="2" t="n">
-        <v>3</v>
-      </c>
       <c r="F53" s="2" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54"/>
@@ -1910,44 +1910,47 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CLASSIC KICK</t>
+          <t>DOOR</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>41 7/8 X 4</t>
+          <t>8 7/8 X 26 1/2</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>47 7/8 X 4</t>
+          <t>11 7/8 X 31 7/8</t>
         </is>
       </c>
       <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>59 7/8 X 4</t>
+          <t>11 7/8 X 26 1/2</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="C6" s="2" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7"/>
@@ -1955,75 +1958,72 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DOOR</t>
+          <t>DRAWER</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>8 7/8 X 26 1/2</t>
-        </is>
+          <t>11 7/8 X 8 3/4</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>15</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>11 7/8 X 31 7/8</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>2</v>
-      </c>
-      <c r="D10" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>11 7/8 X 26 1/2</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="C12" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13"/>
-    <row r="14"/>
+      <c r="C10" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>CLASSIC KICK</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>41 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>47 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+    </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>DRAWER</t>
-        </is>
-      </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>11 7/8 X 8 3/4</t>
+          <t>59 7/8 X 4</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>15</v>
-      </c>
-      <c r="D15" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="C16" s="2" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17"/>
@@ -2131,99 +2131,105 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CLASSIC KICK</t>
+          <t>DOOR</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>14 7/8 X 4</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>1</v>
+          <t>8 7/8 X 26 1/2</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="inlineStr">
         <is>
-          <t>23 7/8 X 4</t>
+          <t>11 7/8 X 26 1/2</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G29" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="inlineStr">
         <is>
-          <t>29 7/8 X 4</t>
-        </is>
-      </c>
-      <c r="E30" t="n">
-        <v>1</v>
+          <t>11 7/8 X 19 1/2</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="inlineStr">
         <is>
-          <t>35 7/8 X 4</t>
-        </is>
-      </c>
-      <c r="G31" t="n">
-        <v>1</v>
+          <t>11 7/8 X 17 9/16</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="inlineStr">
         <is>
-          <t>41 7/8 X 4</t>
-        </is>
-      </c>
-      <c r="H32" t="n">
-        <v>1</v>
+          <t>14 7/8 X 17 9/16</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>4</v>
+      </c>
+      <c r="F32" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="inlineStr">
         <is>
-          <t>59 7/8 X 4</t>
+          <t>14 7/8 X 26 1/2</t>
         </is>
       </c>
       <c r="C33" t="n">
         <v>1</v>
+      </c>
+      <c r="E33" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="inlineStr">
         <is>
-          <t>71 7/8 X 4</t>
+          <t>14 7/8 X 44 1/8</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1</v>
-      </c>
-      <c r="F34" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="C35" s="2" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H35" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36"/>
@@ -2231,194 +2237,188 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>DOOR</t>
+          <t>DRAWER</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>8 7/8 X 26 1/2</t>
-        </is>
+          <t>11 7/8 X 8 3/4</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>6</v>
+      </c>
+      <c r="F38" t="n">
+        <v>3</v>
+      </c>
+      <c r="G38" t="n">
+        <v>3</v>
       </c>
       <c r="H38" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="inlineStr">
         <is>
-          <t>11 7/8 X 17 9/16</t>
+          <t>11 7/8 X 9 11/16</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="inlineStr">
         <is>
-          <t>11 7/8 X 26 1/2</t>
-        </is>
-      </c>
-      <c r="D40" t="n">
-        <v>2</v>
-      </c>
-      <c r="G40" t="n">
+          <t>23 7/8 X 8 3/4</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="inlineStr">
         <is>
-          <t>11 7/8 X 19 1/2</t>
+          <t>29 7/8 X 8 3/4</t>
         </is>
       </c>
       <c r="C41" t="n">
+        <v>2</v>
+      </c>
+      <c r="F41" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="inlineStr">
         <is>
-          <t>14 7/8 X 17 9/16</t>
+          <t>35 7/8 X 6 15/16</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>4</v>
-      </c>
-      <c r="F42" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>14 7/8 X 44 1/8</t>
-        </is>
-      </c>
-      <c r="C43" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>14 7/8 X 26 1/2</t>
-        </is>
-      </c>
-      <c r="C44" t="n">
-        <v>1</v>
-      </c>
-      <c r="E44" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="C45" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="D45" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E45" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F45" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="G45" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="H45" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46"/>
-    <row r="47"/>
+      <c r="C43" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="D43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G43" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H43" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>CLASSIC KICK</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>14 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>23 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>1</v>
+      </c>
+    </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>DRAWER</t>
-        </is>
-      </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>11 7/8 X 9 11/16</t>
-        </is>
-      </c>
-      <c r="C48" t="n">
-        <v>2</v>
+          <t>29 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="inlineStr">
         <is>
-          <t>11 7/8 X 8 3/4</t>
-        </is>
-      </c>
-      <c r="C49" t="n">
-        <v>6</v>
-      </c>
-      <c r="F49" t="n">
-        <v>3</v>
+          <t>35 7/8 X 4</t>
+        </is>
       </c>
       <c r="G49" t="n">
-        <v>3</v>
-      </c>
-      <c r="H49" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="inlineStr">
         <is>
-          <t>23 7/8 X 8 3/4</t>
-        </is>
-      </c>
-      <c r="C50" t="n">
-        <v>2</v>
+          <t>41 7/8 X 4</t>
+        </is>
+      </c>
+      <c r="H50" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="inlineStr">
         <is>
-          <t>29 7/8 X 8 3/4</t>
+          <t>59 7/8 X 4</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2</v>
-      </c>
-      <c r="F51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="inlineStr">
         <is>
-          <t>35 7/8 X 6 15/16</t>
+          <t>71 7/8 X 4</t>
         </is>
       </c>
       <c r="C52" t="n">
+        <v>1</v>
+      </c>
+      <c r="F52" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="53">
       <c r="C53" s="2" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D53" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" s="2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G53" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H53" s="2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54"/>

</xml_diff>